<commit_message>
update and fix bugs
</commit_message>
<xml_diff>
--- a/DoAn/QLTS/wwwroot/Content/files/Import_Equipment.xlsx
+++ b/DoAn/QLTS/wwwroot/Content/files/Import_Equipment.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C26C65-FEEA-4F61-B999-F6EA7B1FE9CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="7632" yWindow="1752" windowWidth="14616" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +49,6 @@
     <t>Macbook Pro 1</t>
   </si>
   <si>
-    <t>0cac181a-474a-11ec-8253-ecf4bb4d36af</t>
-  </si>
-  <si>
     <t>Tốt</t>
   </si>
   <si>
@@ -58,12 +56,15 @@
   </si>
   <si>
     <t>Macbook Pro 2</t>
+  </si>
+  <si>
+    <t>6b38ddb6-1cdc-5f7b-6efa-d9c911cf4972</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -383,11 +384,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,10 +435,10 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -451,16 +452,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
       </c>
       <c r="F3">
         <v>1</v>

</xml_diff>